<commit_message>
update part7 of readme
Signed-off-by: tingyunaiai9 <2920825585@qq.com>
</commit_message>
<xml_diff>
--- a/doc/2024大作业自评表.xlsx
+++ b/doc/2024大作业自评表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\cpp\ProgrammingPractice\QtGame\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6248C668-F9AE-4038-A59F-58A99E1F7A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3982FAEA-09A4-42D8-B6F5-513B98C7DC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -229,74 +229,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -316,7 +248,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CCE8CF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -607,16 +539,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="70.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -632,7 +564,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -640,7 +572,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -648,7 +580,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -656,7 +588,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -664,7 +596,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -672,7 +604,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -712,7 +644,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -720,7 +652,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -728,7 +660,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -736,7 +668,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -752,7 +684,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -768,7 +700,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -776,7 +708,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -784,7 +716,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -792,7 +724,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -800,7 +732,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
@@ -808,7 +740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -821,10 +753,10 @@
         <v>27</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -832,7 +764,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -840,7 +772,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -848,7 +780,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
@@ -856,7 +788,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -864,7 +796,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
@@ -872,7 +804,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -885,10 +817,10 @@
         <v>35</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
@@ -896,7 +828,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
@@ -917,7 +849,7 @@
         <v>39</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="26" x14ac:dyDescent="0.3">
@@ -925,7 +857,7 @@
         <v>40</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="26" x14ac:dyDescent="0.3">
@@ -933,7 +865,7 @@
         <v>41</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="26" x14ac:dyDescent="0.3">
@@ -944,484 +876,484 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B42" s="4"/>
     </row>
-    <row r="43" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B43" s="4"/>
     </row>
-    <row r="44" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B44" s="4"/>
     </row>
-    <row r="45" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B45" s="4"/>
     </row>
-    <row r="46" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B46" s="4"/>
     </row>
-    <row r="47" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B47" s="4"/>
     </row>
-    <row r="48" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B48" s="4"/>
     </row>
-    <row r="49" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" s="4"/>
     </row>
-    <row r="50" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" s="4"/>
     </row>
-    <row r="51" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" s="4"/>
     </row>
-    <row r="52" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" s="4"/>
     </row>
-    <row r="53" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" s="4"/>
     </row>
-    <row r="54" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" s="4"/>
     </row>
-    <row r="55" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" s="4"/>
     </row>
-    <row r="56" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" s="4"/>
     </row>
-    <row r="57" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57" s="4"/>
     </row>
-    <row r="58" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58" s="4"/>
     </row>
-    <row r="59" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" s="4"/>
     </row>
-    <row r="60" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60" s="4"/>
     </row>
-    <row r="61" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61" s="4"/>
     </row>
-    <row r="62" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B62" s="4"/>
     </row>
-    <row r="63" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63" s="4"/>
     </row>
-    <row r="64" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" s="4"/>
     </row>
-    <row r="65" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" s="4"/>
     </row>
-    <row r="66" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" s="4"/>
     </row>
-    <row r="67" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" s="4"/>
     </row>
-    <row r="68" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" s="4"/>
     </row>
-    <row r="69" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" s="4"/>
     </row>
-    <row r="70" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" s="4"/>
     </row>
-    <row r="71" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71" s="4"/>
     </row>
-    <row r="72" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72" s="4"/>
     </row>
-    <row r="73" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73" s="4"/>
     </row>
-    <row r="74" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74" s="4"/>
     </row>
-    <row r="75" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75" s="4"/>
     </row>
-    <row r="76" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B76" s="4"/>
     </row>
-    <row r="77" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B77" s="4"/>
     </row>
-    <row r="78" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B78" s="4"/>
     </row>
-    <row r="79" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79" s="4"/>
     </row>
-    <row r="80" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80" s="4"/>
     </row>
-    <row r="81" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="4"/>
     </row>
-    <row r="82" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" s="4"/>
     </row>
-    <row r="83" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="4"/>
     </row>
-    <row r="84" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="4"/>
     </row>
-    <row r="85" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="4"/>
     </row>
-    <row r="86" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="4"/>
     </row>
-    <row r="87" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87" s="4"/>
     </row>
-    <row r="88" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88" s="4"/>
     </row>
-    <row r="89" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" s="4"/>
     </row>
-    <row r="90" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="4"/>
     </row>
-    <row r="91" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="4"/>
     </row>
-    <row r="92" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92" s="4"/>
     </row>
-    <row r="93" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93" s="4"/>
     </row>
-    <row r="94" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B94" s="4"/>
     </row>
-    <row r="95" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B95" s="4"/>
     </row>
-    <row r="96" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B96" s="4"/>
     </row>
-    <row r="97" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B97" s="4"/>
     </row>
-    <row r="98" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" s="4"/>
     </row>
-    <row r="99" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B99" s="4"/>
     </row>
-    <row r="100" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B100" s="4"/>
     </row>
-    <row r="101" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B101" s="4"/>
     </row>
-    <row r="102" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B102" s="4"/>
     </row>
-    <row r="103" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B103" s="4"/>
     </row>
-    <row r="104" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B104" s="4"/>
     </row>
-    <row r="105" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B105" s="4"/>
     </row>
-    <row r="106" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B106" s="4"/>
     </row>
-    <row r="107" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B107" s="4"/>
     </row>
-    <row r="108" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B108" s="4"/>
     </row>
-    <row r="109" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B109" s="4"/>
     </row>
-    <row r="110" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B110" s="4"/>
     </row>
-    <row r="111" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B111" s="4"/>
     </row>
-    <row r="112" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B112" s="4"/>
     </row>
-    <row r="113" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B113" s="4"/>
     </row>
-    <row r="114" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B114" s="4"/>
     </row>
-    <row r="115" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B115" s="4"/>
     </row>
-    <row r="116" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B116" s="4"/>
     </row>
-    <row r="117" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B117" s="4"/>
     </row>
-    <row r="118" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B118" s="4"/>
     </row>
-    <row r="119" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B119" s="4"/>
     </row>
-    <row r="120" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B120" s="4"/>
     </row>
-    <row r="121" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B121" s="4"/>
     </row>
-    <row r="122" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B122" s="4"/>
     </row>
-    <row r="123" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B123" s="4"/>
     </row>
-    <row r="124" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B124" s="4"/>
     </row>
-    <row r="125" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B125" s="4"/>
     </row>
-    <row r="126" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B126" s="4"/>
     </row>
-    <row r="127" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B127" s="4"/>
     </row>
-    <row r="128" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B128" s="4"/>
     </row>
-    <row r="129" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B129" s="4"/>
     </row>
-    <row r="130" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B130" s="4"/>
     </row>
-    <row r="131" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B131" s="4"/>
     </row>
-    <row r="132" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B132" s="4"/>
     </row>
-    <row r="133" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B133" s="4"/>
     </row>
-    <row r="134" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B134" s="4"/>
     </row>
-    <row r="135" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B135" s="4"/>
     </row>
-    <row r="136" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B136" s="4"/>
     </row>
-    <row r="137" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B137" s="4"/>
     </row>
-    <row r="138" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B138" s="4"/>
     </row>
-    <row r="139" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B139" s="4"/>
     </row>
-    <row r="140" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B140" s="4"/>
     </row>
-    <row r="141" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B141" s="4"/>
     </row>
-    <row r="142" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B142" s="4"/>
     </row>
-    <row r="143" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B143" s="4"/>
     </row>
-    <row r="144" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B144" s="4"/>
     </row>
-    <row r="145" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B145" s="4"/>
     </row>
-    <row r="146" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B146" s="4"/>
     </row>
-    <row r="147" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B147" s="4"/>
     </row>
-    <row r="148" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B148" s="4"/>
     </row>
-    <row r="149" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B149" s="4"/>
     </row>
-    <row r="150" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B150" s="4"/>
     </row>
-    <row r="151" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B151" s="4"/>
     </row>
-    <row r="152" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B152" s="4"/>
     </row>
-    <row r="153" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B153" s="4"/>
     </row>
-    <row r="154" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B154" s="4"/>
     </row>
-    <row r="155" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B155" s="4"/>
     </row>
-    <row r="156" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B156" s="4"/>
     </row>
-    <row r="157" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B157" s="4"/>
     </row>
-    <row r="158" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B158" s="4"/>
     </row>
-    <row r="159" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B159" s="4"/>
     </row>
-    <row r="160" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B160" s="4"/>
     </row>
-    <row r="161" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B161" s="4"/>
     </row>
-    <row r="162" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B162" s="4"/>
     </row>
-    <row r="163" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B163" s="4"/>
     </row>
-    <row r="164" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B164" s="4"/>
     </row>
-    <row r="165" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B165" s="4"/>
     </row>
-    <row r="166" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B166" s="4"/>
     </row>
-    <row r="167" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B167" s="4"/>
     </row>
-    <row r="168" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B168" s="4"/>
     </row>
-    <row r="169" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B169" s="4"/>
     </row>
-    <row r="170" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B170" s="4"/>
     </row>
-    <row r="171" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B171" s="4"/>
     </row>
-    <row r="172" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B172" s="4"/>
     </row>
-    <row r="173" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B173" s="4"/>
     </row>
-    <row r="174" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B174" s="4"/>
     </row>
-    <row r="175" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B175" s="4"/>
     </row>
-    <row r="176" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B176" s="4"/>
     </row>
-    <row r="177" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B177" s="4"/>
     </row>
-    <row r="178" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B178" s="4"/>
     </row>
-    <row r="179" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B179" s="4"/>
     </row>
-    <row r="180" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B180" s="4"/>
     </row>
-    <row r="181" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B181" s="4"/>
     </row>
-    <row r="182" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B182" s="4"/>
     </row>
-    <row r="183" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B183" s="4"/>
     </row>
-    <row r="184" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B184" s="4"/>
     </row>
-    <row r="185" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B185" s="4"/>
     </row>
-    <row r="186" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B186" s="4"/>
     </row>
-    <row r="187" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B187" s="4"/>
     </row>
-    <row r="188" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B188" s="4"/>
     </row>
-    <row r="189" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B189" s="4"/>
     </row>
-    <row r="190" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B190" s="4"/>
     </row>
-    <row r="191" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B191" s="4"/>
     </row>
-    <row r="192" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B192" s="4"/>
     </row>
-    <row r="193" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B193" s="4"/>
     </row>
-    <row r="194" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B194" s="4"/>
     </row>
-    <row r="195" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B195" s="4"/>
     </row>
-    <row r="196" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B196" s="4"/>
     </row>
-    <row r="197" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B197" s="4"/>
     </row>
-    <row r="198" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B198" s="4"/>
     </row>
-    <row r="199" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B199" s="4"/>
     </row>
-    <row r="200" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B200" s="4"/>
     </row>
-    <row r="201" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B201" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify part 7.9-7.11 of readme
Signed-off-by: tingyunaiai9 <2920825585@qq.com>
</commit_message>
<xml_diff>
--- a/doc/2024大作业自评表.xlsx
+++ b/doc/2024大作业自评表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\cpp\ProgrammingPractice\QtGame\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3982FAEA-09A4-42D8-B6F5-513B98C7DC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718AF26E-08BD-4FE7-A3A1-C8EEFB2E9915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -737,7 +737,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>